<commit_message>
EPBDS-12588 The columns with true conditions are matched with output object, if the number of IsTrue conditions>8
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-10143_SmartRules_With_Collect.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-10143_SmartRules_With_Collect.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\demo\openl-demo\user-workspace\DEFAULT\Collect2Darray\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA86800-26AB-4819-B1B8-EE5EC3845056}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F807863C-5D9A-4BF2-B84B-5B27AB552CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7470" yWindow="420" windowWidth="27090" windowHeight="13995" xr2:uid="{AF2CC9EF-E362-41FF-8D1B-84F4EE5BB9C0}"/>
+    <workbookView xWindow="7740" yWindow="1515" windowWidth="19080" windowHeight="12600" xr2:uid="{AF2CC9EF-E362-41FF-8D1B-84F4EE5BB9C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
   <si>
     <t>Datatype Package</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>SmartRules Collect Package[] pack_rule2()</t>
-  </si>
-  <si>
-    <t>SmartRules Collect Package[][] main_rule(String cond)</t>
   </si>
   <si>
     <t>TEST</t>
@@ -102,11 +99,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -131,7 +127,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -453,20 +449,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A43047A4-D990-425F-A3EC-17A9D8B96F73}">
-  <dimension ref="B4:D40"/>
+  <dimension ref="B4:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -474,7 +470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -482,110 +478,86 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
       </c>
-      <c r="D13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
       </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
       </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>2</v>
       </c>
       <c r="C20" t="s">
         <v>3</v>
       </c>
-      <c r="D20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>7</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
-      <c r="D21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>8</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>10</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
       </c>
-      <c r="D23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>4</v>
       </c>
@@ -593,53 +565,47 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>2</v>
       </c>
       <c r="C32" t="s">
         <v>3</v>
       </c>
-      <c r="D32" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>7</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
       </c>
-      <c r="D33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>4</v>
       </c>
@@ -647,18 +613,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>